<commit_message>
Fixed Attendance import script
</commit_message>
<xml_diff>
--- a/excel/Attendance.xlsx
+++ b/excel/Attendance.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Week No</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Classes Held</t>
   </si>
   <si>
-    <t>Classes Attend</t>
+    <t>Classes Attended</t>
   </si>
   <si>
     <t>A</t>
@@ -80,9 +80,6 @@
     <t>10me56</t>
   </si>
   <si>
-    <t>1ru78678</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -92,13 +89,13 @@
     <t>12cs42</t>
   </si>
   <si>
+    <t>1ru236</t>
+  </si>
+  <si>
     <t>MS</t>
   </si>
   <si>
     <t>12cs03</t>
-  </si>
-  <si>
-    <t>1ru3453</t>
   </si>
 </sst>
 </file>
@@ -113,6 +110,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -196,13 +194,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -268,7 +266,7 @@
       <c r="G2" s="0" t="n">
         <v>2014</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -300,7 +298,7 @@
       <c r="G3" s="0" t="n">
         <v>2012</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="0" t="n">
@@ -312,7 +310,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
@@ -332,8 +330,8 @@
       <c r="G4" s="0" t="n">
         <v>2013</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
+      <c r="H4" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>26</v>
@@ -344,28 +342,28 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2014</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>13</v>
+      <c r="H5" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>30</v>
@@ -376,7 +374,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5</v>
@@ -396,8 +394,8 @@
       <c r="G6" s="0" t="n">
         <v>2012</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
+      <c r="H6" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>33</v>

</xml_diff>

<commit_message>
Modified example excel files to meet integrity constraints, removed composite key in WeeklyAttendance
</commit_message>
<xml_diff>
--- a/excel/Attendance.xlsx
+++ b/excel/Attendance.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Week No</t>
   </si>
@@ -56,46 +56,16 @@
     <t>10cs42</t>
   </si>
   <si>
-    <t>1ru233</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>BTECH</t>
-  </si>
-  <si>
-    <t>10ec45</t>
-  </si>
-  <si>
-    <t>1ru56456</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>10me56</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>MTECH</t>
-  </si>
-  <si>
-    <t>12cs42</t>
-  </si>
-  <si>
-    <t>1ru236</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>12cs03</t>
+    <t>1ru353</t>
+  </si>
+  <si>
+    <t>10cs48</t>
+  </si>
+  <si>
+    <t>10cs49</t>
+  </si>
+  <si>
+    <t>10cs50</t>
   </si>
 </sst>
 </file>
@@ -200,7 +170,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -281,25 +251,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>20</v>
@@ -310,25 +280,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>13</v>
@@ -342,28 +312,28 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>30</v>
@@ -374,7 +344,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5</v>
@@ -383,19 +353,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>33</v>

</xml_diff>